<commit_message>
feat(data): cleaning and gnerating other notebooks
</commit_message>
<xml_diff>
--- a/src/data/RIASEC_words.xlsx
+++ b/src/data/RIASEC_words.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ariannakazemi/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vunl-my.sharepoint.com/personal/l_morabito_vu_nl/Documents/Desktop/vita-vu.github.io/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9693F3D9-6BAD-FF4B-85E5-5BBC12C132E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{9693F3D9-6BAD-FF4B-85E5-5BBC12C132E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B524EA5B-2529-4872-B6FF-E485158A1839}"/>
   <bookViews>
-    <workbookView xWindow="-18020" yWindow="-20720" windowWidth="26920" windowHeight="16240" xr2:uid="{F36EE09E-CAF0-C040-93B8-6CC46F9506A9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{F36EE09E-CAF0-C040-93B8-6CC46F9506A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -561,7 +561,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -578,6 +578,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -600,14 +608,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -942,17 +953,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B3BB1AA-F4E0-7242-A063-BD459073B4C1}">
   <dimension ref="A1:D122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="D127" sqref="D127"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="D94" sqref="D94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="18.1640625" customWidth="1"/>
     <col min="4" max="4" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -966,7 +977,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -980,7 +991,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -994,7 +1005,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1008,7 +1019,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1022,7 +1033,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1036,7 +1047,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -1050,7 +1061,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -1064,7 +1075,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
@@ -1078,7 +1089,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
@@ -1092,7 +1103,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1106,7 +1117,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
@@ -1120,7 +1131,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
@@ -1134,7 +1145,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
@@ -1148,7 +1159,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -1162,7 +1173,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
@@ -1176,7 +1187,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
@@ -1190,7 +1201,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
@@ -1200,11 +1211,11 @@
       <c r="C18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
         <v>5</v>
       </c>
@@ -1218,7 +1229,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
         <v>5</v>
       </c>
@@ -1232,7 +1243,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
@@ -1246,7 +1257,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
         <v>5</v>
       </c>
@@ -1260,7 +1271,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
         <v>6</v>
       </c>
@@ -1274,7 +1285,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
@@ -1288,7 +1299,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
         <v>6</v>
       </c>
@@ -1302,7 +1313,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
@@ -1316,7 +1327,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
         <v>6</v>
       </c>
@@ -1330,7 +1341,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
         <v>6</v>
       </c>
@@ -1344,7 +1355,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
         <v>6</v>
       </c>
@@ -1358,7 +1369,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A30" s="1" t="s">
         <v>6</v>
       </c>
@@ -1372,7 +1383,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
         <v>7</v>
       </c>
@@ -1386,7 +1397,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
         <v>7</v>
       </c>
@@ -1400,7 +1411,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A33" s="1" t="s">
         <v>7</v>
       </c>
@@ -1414,7 +1425,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A34" s="1" t="s">
         <v>7</v>
       </c>
@@ -1428,7 +1439,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A35" s="1" t="s">
         <v>7</v>
       </c>
@@ -1442,7 +1453,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
         <v>7</v>
       </c>
@@ -1456,7 +1467,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A37" s="1" t="s">
         <v>7</v>
       </c>
@@ -1470,7 +1481,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A38" s="1" t="s">
         <v>7</v>
       </c>
@@ -1484,7 +1495,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A39" s="1" t="s">
         <v>8</v>
       </c>
@@ -1498,7 +1509,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A40" s="1" t="s">
         <v>8</v>
       </c>
@@ -1512,7 +1523,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A41" s="1" t="s">
         <v>8</v>
       </c>
@@ -1526,7 +1537,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A42" s="1" t="s">
         <v>8</v>
       </c>
@@ -1540,7 +1551,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A43" s="1" t="s">
         <v>8</v>
       </c>
@@ -1554,7 +1565,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A44" s="1" t="s">
         <v>8</v>
       </c>
@@ -1568,7 +1579,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A45" s="1" t="s">
         <v>8</v>
       </c>
@@ -1582,7 +1593,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A46" s="1" t="s">
         <v>8</v>
       </c>
@@ -1596,7 +1607,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A47" s="1" t="s">
         <v>3</v>
       </c>
@@ -1610,7 +1621,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A48" s="1" t="s">
         <v>3</v>
       </c>
@@ -1624,7 +1635,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A49" s="1" t="s">
         <v>3</v>
       </c>
@@ -1638,7 +1649,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A50" s="1" t="s">
         <v>3</v>
       </c>
@@ -1652,7 +1663,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A51" s="1" t="s">
         <v>3</v>
       </c>
@@ -1666,7 +1677,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A52" s="1" t="s">
         <v>3</v>
       </c>
@@ -1680,7 +1691,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A53" s="1" t="s">
         <v>4</v>
       </c>
@@ -1694,7 +1705,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A54" s="1" t="s">
         <v>4</v>
       </c>
@@ -1708,7 +1719,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A55" s="1" t="s">
         <v>4</v>
       </c>
@@ -1722,7 +1733,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A56" s="1" t="s">
         <v>4</v>
       </c>
@@ -1736,7 +1747,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A57" s="1" t="s">
         <v>4</v>
       </c>
@@ -1750,7 +1761,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A58" s="1" t="s">
         <v>4</v>
       </c>
@@ -1764,7 +1775,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A59" s="1" t="s">
         <v>4</v>
       </c>
@@ -1778,7 +1789,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A60" s="1" t="s">
         <v>4</v>
       </c>
@@ -1792,7 +1803,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A61" s="1" t="s">
         <v>4</v>
       </c>
@@ -1806,7 +1817,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A62" s="1" t="s">
         <v>5</v>
       </c>
@@ -1820,7 +1831,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A63" s="1" t="s">
         <v>5</v>
       </c>
@@ -1834,7 +1845,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A64" s="1" t="s">
         <v>5</v>
       </c>
@@ -1848,7 +1859,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A65" s="1" t="s">
         <v>5</v>
       </c>
@@ -1862,7 +1873,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A66" s="1" t="s">
         <v>5</v>
       </c>
@@ -1876,7 +1887,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A67" s="1" t="s">
         <v>5</v>
       </c>
@@ -1890,7 +1901,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A68" s="1" t="s">
         <v>5</v>
       </c>
@@ -1904,7 +1915,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A69" s="1" t="s">
         <v>4</v>
       </c>
@@ -1918,7 +1929,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A70" s="1" t="s">
         <v>4</v>
       </c>
@@ -1932,7 +1943,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A71" s="1" t="s">
         <v>4</v>
       </c>
@@ -1946,7 +1957,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A72" s="1" t="s">
         <v>4</v>
       </c>
@@ -1960,7 +1971,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A73" s="1" t="s">
         <v>3</v>
       </c>
@@ -1974,7 +1985,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A74" s="1" t="s">
         <v>3</v>
       </c>
@@ -1988,7 +1999,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A75" s="1" t="s">
         <v>3</v>
       </c>
@@ -2002,7 +2013,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A76" s="1" t="s">
         <v>3</v>
       </c>
@@ -2016,7 +2027,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A77" s="1" t="s">
         <v>3</v>
       </c>
@@ -2030,7 +2041,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A78" s="1" t="s">
         <v>3</v>
       </c>
@@ -2044,7 +2055,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A79" s="1" t="s">
         <v>3</v>
       </c>
@@ -2058,7 +2069,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A80" s="1" t="s">
         <v>3</v>
       </c>
@@ -2072,7 +2083,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A81" s="1" t="s">
         <v>5</v>
       </c>
@@ -2086,7 +2097,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A82" s="1" t="s">
         <v>5</v>
       </c>
@@ -2100,7 +2111,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A83" s="1" t="s">
         <v>5</v>
       </c>
@@ -2114,7 +2125,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A84" s="1" t="s">
         <v>5</v>
       </c>
@@ -2128,7 +2139,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A85" s="1" t="s">
         <v>5</v>
       </c>
@@ -2142,7 +2153,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A86" s="1" t="s">
         <v>6</v>
       </c>
@@ -2156,7 +2167,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A87" s="1" t="s">
         <v>6</v>
       </c>
@@ -2170,7 +2181,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A88" s="1" t="s">
         <v>6</v>
       </c>
@@ -2184,7 +2195,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A89" s="1" t="s">
         <v>6</v>
       </c>
@@ -2198,7 +2209,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A90" s="1" t="s">
         <v>6</v>
       </c>
@@ -2212,7 +2223,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A91" s="1" t="s">
         <v>6</v>
       </c>
@@ -2226,7 +2237,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A92" s="1" t="s">
         <v>6</v>
       </c>
@@ -2240,7 +2251,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A93" s="1" t="s">
         <v>6</v>
       </c>
@@ -2254,7 +2265,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A94" s="1" t="s">
         <v>6</v>
       </c>
@@ -2268,7 +2279,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A95" s="1" t="s">
         <v>6</v>
       </c>
@@ -2282,7 +2293,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A96" s="1" t="s">
         <v>6</v>
       </c>
@@ -2296,7 +2307,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A97" s="1" t="s">
         <v>7</v>
       </c>
@@ -2310,7 +2321,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A98" s="1" t="s">
         <v>7</v>
       </c>
@@ -2324,7 +2335,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A99" s="1" t="s">
         <v>7</v>
       </c>
@@ -2338,7 +2349,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A100" s="1" t="s">
         <v>7</v>
       </c>
@@ -2352,7 +2363,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A101" s="1" t="s">
         <v>7</v>
       </c>
@@ -2366,7 +2377,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A102" s="1" t="s">
         <v>7</v>
       </c>
@@ -2380,7 +2391,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A103" s="1" t="s">
         <v>7</v>
       </c>
@@ -2394,7 +2405,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A104" s="1" t="s">
         <v>7</v>
       </c>
@@ -2408,7 +2419,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A105" s="1" t="s">
         <v>7</v>
       </c>
@@ -2422,7 +2433,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A106" s="1" t="s">
         <v>7</v>
       </c>
@@ -2436,7 +2447,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A107" s="1" t="s">
         <v>7</v>
       </c>
@@ -2450,7 +2461,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A108" s="1" t="s">
         <v>7</v>
       </c>
@@ -2464,7 +2475,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A109" s="1" t="s">
         <v>7</v>
       </c>
@@ -2478,7 +2489,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A110" s="1" t="s">
         <v>8</v>
       </c>
@@ -2492,7 +2503,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A111" s="1" t="s">
         <v>8</v>
       </c>
@@ -2506,7 +2517,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A112" s="1" t="s">
         <v>8</v>
       </c>
@@ -2520,7 +2531,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A113" s="1" t="s">
         <v>8</v>
       </c>
@@ -2534,7 +2545,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A114" s="1" t="s">
         <v>8</v>
       </c>
@@ -2548,7 +2559,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A115" s="1" t="s">
         <v>8</v>
       </c>
@@ -2562,7 +2573,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A116" s="1" t="s">
         <v>8</v>
       </c>
@@ -2576,7 +2587,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A117" s="1" t="s">
         <v>8</v>
       </c>
@@ -2590,7 +2601,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A118" s="1" t="s">
         <v>8</v>
       </c>
@@ -2604,7 +2615,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A119" s="1" t="s">
         <v>8</v>
       </c>
@@ -2618,7 +2629,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A120" s="1" t="s">
         <v>8</v>
       </c>
@@ -2632,7 +2643,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A121" s="1" t="s">
         <v>8</v>
       </c>
@@ -2646,7 +2657,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A122" s="1" t="s">
         <v>8</v>
       </c>
@@ -2662,6 +2673,9 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D18" r:id="rId1" xr:uid="{020C34D2-993E-48C9-83CA-92CE7263910A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>